<commit_message>
se agrega hasta domingo noche
</commit_message>
<xml_diff>
--- a/public/exports/Usuario_formatoGV.xlsx
+++ b/public/exports/Usuario_formatoGV.xlsx
@@ -19,9 +19,6 @@
     <t>REPORTE POR USUARIO</t>
   </si>
   <si>
-    <t>Número de Documento</t>
-  </si>
-  <si>
     <t>Nombre de Documento</t>
   </si>
   <si>
@@ -32,6 +29,9 @@
   </si>
   <si>
     <t>Motivo</t>
+  </si>
+  <si>
+    <t>Cliente</t>
   </si>
 </sst>
 </file>
@@ -509,14 +509,14 @@
   <dimension ref="C2:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:G2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" style="6" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" style="6" customWidth="1"/>
@@ -556,21 +556,21 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="6" spans="3:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>